<commit_message>
Pak Read/Write Communication Implemented! Both reading from and writing to a pak device is working (only Controller Pak tested but others should work too). Migration complete and beneficial.
Signed-off-by: bigbass1997 <bigbass1997.website@gmail.com>
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="121">
   <si>
     <t>PORTA</t>
   </si>
@@ -94,12 +94,6 @@
     <t>MEM_RW</t>
   </si>
   <si>
-    <t>ADDR_SER</t>
-  </si>
-  <si>
-    <t>ADDR_CLK</t>
-  </si>
-  <si>
     <t>IO_CLK</t>
   </si>
   <si>
@@ -377,6 +371,18 @@
   </si>
   <si>
     <t>UART2 TX</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>SDO</t>
+  </si>
+  <si>
+    <t>SPI1 TX</t>
+  </si>
+  <si>
+    <t>ADDR_LAT</t>
   </si>
 </sst>
 </file>
@@ -678,6 +684,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -689,9 +698,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,7 +993,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1009,69 +1015,69 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="29"/>
+        <v>29</v>
+      </c>
+      <c r="F1" s="25"/>
       <c r="G1" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="O1" s="26"/>
+        <v>115</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="15">
         <v>1</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>108</v>
+      <c r="F2" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="G2" s="15">
         <v>40</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K2" s="15"/>
       <c r="N2" s="18" t="s">
@@ -1082,29 +1088,29 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" s="18">
         <v>2</v>
       </c>
-      <c r="F3" s="25"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="15">
         <v>39</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K3" s="15"/>
       <c r="N3" s="17" t="s">
@@ -1115,32 +1121,32 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" s="18">
         <v>3</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="17">
         <v>38</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N4" s="19" t="s">
         <v>2</v>
@@ -1150,29 +1156,29 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5" s="18">
         <v>4</v>
       </c>
-      <c r="F5" s="25"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="17">
         <v>37</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K5" s="17"/>
       <c r="N5" s="20" t="s">
@@ -1183,29 +1189,29 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E6" s="18">
         <v>5</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="17">
         <v>36</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K6" s="17"/>
       <c r="N6" s="21" t="s">
@@ -1216,114 +1222,120 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E7" s="18">
         <v>6</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="17">
         <v>35</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K7" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="N7" s="15" t="s">
-        <v>112</v>
       </c>
       <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8" s="18">
         <v>7</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="17">
         <v>34</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+        <v>91</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="21">
         <v>8</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="17">
         <v>33</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="21">
         <v>9</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="26"/>
       <c r="G10" s="23">
         <v>32</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
@@ -1332,23 +1344,23 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E11" s="21">
         <v>10</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="22">
         <v>31</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
@@ -1359,66 +1371,74 @@
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E12" s="23">
         <v>11</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="20">
         <v>30</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
+        <v>93</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E13" s="22">
         <v>12</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="20">
         <v>29</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
+        <v>94</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E14" s="18">
         <v>13</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="20">
         <v>28</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>114</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1426,197 +1446,193 @@
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E15" s="18">
         <v>14</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="20">
         <v>27</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>114</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
       <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="19">
         <v>15</v>
       </c>
-      <c r="F16" s="25"/>
+      <c r="F16" s="26"/>
       <c r="G16" s="19">
         <v>26</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>23</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E17" s="19">
         <v>16</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="26"/>
       <c r="G17" s="19">
         <v>25</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" s="19">
         <v>17</v>
       </c>
-      <c r="F18" s="25"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="19">
         <v>24</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E19" s="19">
         <v>18</v>
       </c>
-      <c r="F19" s="25"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="19">
         <v>23</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E20" s="20">
         <v>19</v>
       </c>
-      <c r="F20" s="25"/>
+      <c r="F20" s="26"/>
       <c r="G20" s="20">
         <v>22</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E21" s="20">
         <v>20</v>
       </c>
-      <c r="F21" s="25"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="20">
         <v>21</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K21" s="20"/>
     </row>
@@ -1648,83 +1664,83 @@
     <row r="1" spans="2:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
+        <v>60</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="O3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="Q3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3">
         <v>32</v>
@@ -1777,26 +1793,26 @@
     </row>
     <row r="5" spans="2:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3">
         <v>16</v>
@@ -1849,79 +1865,79 @@
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
+        <v>60</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Controller Pak fails to communicate, some WIP code to debug this; possibly has something to do with CE pin always being held LOW.
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="Microcontroller" sheetId="6" r:id="rId1"/>
-    <sheet name="Accessory PAKs" sheetId="4" r:id="rId2"/>
+    <sheet name="Accessory Paks" sheetId="4" r:id="rId2"/>
+    <sheet name="Transfer Pak Ribbon" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="125">
   <si>
     <t>PORTA</t>
   </si>
@@ -91,9 +92,6 @@
     <t>DATA_IO</t>
   </si>
   <si>
-    <t>MEM_RW</t>
-  </si>
-  <si>
     <t>IO_CLK</t>
   </si>
   <si>
@@ -136,9 +134,6 @@
     <t>A10</t>
   </si>
   <si>
-    <t>OE</t>
-  </si>
-  <si>
     <t>A11</t>
   </si>
   <si>
@@ -211,9 +206,6 @@
     <t>IO_OE1</t>
   </si>
   <si>
-    <t>WE</t>
-  </si>
-  <si>
     <t>Usage</t>
   </si>
   <si>
@@ -383,6 +375,27 @@
   </si>
   <si>
     <t>ADDR_LAT</t>
+  </si>
+  <si>
+    <t>Gameboy Slot</t>
+  </si>
+  <si>
+    <t>Ribbon Cable from Pak Connector</t>
+  </si>
+  <si>
+    <t>Top Face of Transfer Pak PCB</t>
+  </si>
+  <si>
+    <t>/OE</t>
+  </si>
+  <si>
+    <t>/WE</t>
+  </si>
+  <si>
+    <t>PAK_RW</t>
+  </si>
+  <si>
+    <t>PAK_OE</t>
   </si>
 </sst>
 </file>
@@ -610,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -687,6 +700,9 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -697,6 +713,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -993,7 +1012,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1015,69 +1034,69 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="25"/>
       <c r="G1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>30</v>
-      </c>
       <c r="I1" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="O1" s="27"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" s="15">
         <v>1</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>106</v>
+      <c r="F2" s="27" t="s">
+        <v>103</v>
       </c>
       <c r="G2" s="15">
         <v>40</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K2" s="15"/>
       <c r="N2" s="18" t="s">
@@ -1088,29 +1107,29 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E3" s="18">
         <v>2</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="15">
         <v>39</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K3" s="15"/>
       <c r="N3" s="17" t="s">
@@ -1121,32 +1140,32 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" s="18">
         <v>3</v>
       </c>
-      <c r="F4" s="26"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="17">
         <v>38</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N4" s="19" t="s">
         <v>2</v>
@@ -1156,29 +1175,29 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E5" s="18">
         <v>4</v>
       </c>
-      <c r="F5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="17">
         <v>37</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K5" s="17"/>
       <c r="N5" s="20" t="s">
@@ -1189,29 +1208,29 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E6" s="18">
         <v>5</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="17">
         <v>36</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K6" s="17"/>
       <c r="N6" s="21" t="s">
@@ -1222,120 +1241,120 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E7" s="18">
         <v>6</v>
       </c>
-      <c r="F7" s="26"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="17">
         <v>35</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E8" s="18">
         <v>7</v>
       </c>
-      <c r="F8" s="26"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="17">
         <v>34</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E9" s="21">
         <v>8</v>
       </c>
-      <c r="F9" s="26"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="17">
         <v>33</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E10" s="21">
         <v>9</v>
       </c>
-      <c r="F10" s="26"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="23">
         <v>32</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
@@ -1344,23 +1363,23 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E11" s="21">
         <v>10</v>
       </c>
-      <c r="F11" s="26"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="22">
         <v>31</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
@@ -1371,26 +1390,26 @@
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E12" s="23">
         <v>11</v>
       </c>
-      <c r="F12" s="26"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="20">
         <v>30</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I12" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="J12" s="20" t="s">
-        <v>112</v>
-      </c>
       <c r="K12" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1398,26 +1417,26 @@
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" s="22">
         <v>12</v>
       </c>
-      <c r="F13" s="26"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="20">
         <v>29</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1425,17 +1444,17 @@
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" s="18">
         <v>13</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="20">
         <v>28</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -1446,193 +1465,197 @@
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E15" s="18">
         <v>14</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="20">
         <v>27</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
+        <v>93</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E16" s="19">
         <v>15</v>
       </c>
-      <c r="F16" s="26"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="19">
         <v>26</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E17" s="19">
         <v>16</v>
       </c>
-      <c r="F17" s="26"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="19">
         <v>25</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E18" s="19">
         <v>17</v>
       </c>
-      <c r="F18" s="26"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="19">
         <v>24</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E19" s="19">
         <v>18</v>
       </c>
-      <c r="F19" s="26"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="19">
         <v>23</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E20" s="20">
         <v>19</v>
       </c>
-      <c r="F20" s="26"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="20">
         <v>22</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E21" s="20">
         <v>20</v>
       </c>
-      <c r="F21" s="26"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="20">
         <v>21</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K21" s="20"/>
     </row>
@@ -1652,7 +1675,7 @@
   <dimension ref="B1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,83 +1687,83 @@
     <row r="1" spans="2:18" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
+        <v>58</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="O3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="Q3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3">
         <v>32</v>
@@ -1793,26 +1816,26 @@
     </row>
     <row r="5" spans="2:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3">
         <v>16</v>
@@ -1865,79 +1888,79 @@
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
+        <v>58</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1947,4 +1970,344 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AG6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="32" width="5.85546875" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26"/>
+      <c r="C3" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="31"/>
+      <c r="AG3" s="26"/>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="9">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3">
+        <v>25</v>
+      </c>
+      <c r="I4" s="3">
+        <v>24</v>
+      </c>
+      <c r="J4" s="3">
+        <v>23</v>
+      </c>
+      <c r="K4" s="3">
+        <v>22</v>
+      </c>
+      <c r="L4" s="3">
+        <v>21</v>
+      </c>
+      <c r="M4" s="5">
+        <v>20</v>
+      </c>
+      <c r="N4" s="5">
+        <v>19</v>
+      </c>
+      <c r="O4" s="5">
+        <v>18</v>
+      </c>
+      <c r="P4" s="6">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>16</v>
+      </c>
+      <c r="R4" s="5">
+        <v>15</v>
+      </c>
+      <c r="S4" s="5">
+        <v>14</v>
+      </c>
+      <c r="T4" s="5">
+        <v>13</v>
+      </c>
+      <c r="U4" s="5">
+        <v>12</v>
+      </c>
+      <c r="V4" s="5">
+        <v>11</v>
+      </c>
+      <c r="W4" s="5">
+        <v>10</v>
+      </c>
+      <c r="X4" s="5">
+        <v>9</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>7</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>6</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="8">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:AF2"/>
+    <mergeCell ref="C3:AF3"/>
+    <mergeCell ref="C6:AF6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>